<commit_message>
Update test case reference files. The order of elements in /docProps/app.xml has changed.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/ConditionalFormatting/CFDataBar.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/ConditionalFormatting/CFDataBar.xlsx
@@ -399,7 +399,7 @@
       </x:dataBar>
       <x:extLst>
         <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0cf7a109-a037-492e-9fee-4b588b6e219c}</x14:id>
+          <x14:id>{d93cbe18-200b-4d47-80c5-cb2c911c7530}</x14:id>
         </x:ext>
       </x:extLst>
     </x:cfRule>
@@ -413,7 +413,7 @@
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0cf7a109-a037-492e-9fee-4b588b6e219c}">
+          <x14:cfRule type="dataBar" id="{d93cbe18-200b-4d47-80c5-cb2c911c7530}">
             <x14:dataBar minLength="0" maxLength="100" showValue="0" gradient="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
Fiddeling with machine specific behavior
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/ConditionalFormatting/CFDataBar.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/ConditionalFormatting/CFDataBar.xlsx
@@ -399,7 +399,7 @@
       </x:dataBar>
       <x:extLst>
         <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2de8ab59-7976-40e4-8dc9-5ff036098076}</x14:id>
+          <x14:id>{4a4a7953-20a3-4718-a1ce-a4d8fb63b33e}</x14:id>
         </x:ext>
       </x:extLst>
     </x:cfRule>
@@ -413,7 +413,7 @@
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2de8ab59-7976-40e4-8dc9-5ff036098076}">
+          <x14:cfRule type="dataBar" id="{4a4a7953-20a3-4718-a1ce-a4d8fb63b33e}">
             <x14:dataBar minLength="0" maxLength="100" showValue="0" gradient="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
9/9 Saving SheeData through streaming: Remove orphan deletion that hydrates whole Worksheet after it has been saved through streaming by accessing the worksheetPart.Worksheet property (that property automatically hydrates whole worksheet). We don't need to delete orphans, because it is already done in GenerateWorksheetPartContent (though it should be moved later into first phase of saving).
The attached hydrated worksheet saved namespaces slighlyt differently (same namespace prefix was used at multiple place in a tree), so update test files. Not actual change.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/ConditionalFormatting/CFDataBar.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/ConditionalFormatting/CFDataBar.xlsx
@@ -359,7 +359,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -399,7 +399,7 @@
       </x:dataBar>
       <x:extLst>
         <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{d93cbe18-200b-4d47-80c5-cb2c911c7530}</x14:id>
+          <x14:id>{03b9cbb7-aa24-4b4a-9259-410e0ad5897e}</x14:id>
         </x:ext>
       </x:extLst>
     </x:cfRule>
@@ -413,7 +413,7 @@
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{d93cbe18-200b-4d47-80c5-cb2c911c7530}">
+          <x14:cfRule type="dataBar" id="{03b9cbb7-aa24-4b4a-9259-410e0ad5897e}">
             <x14:dataBar minLength="0" maxLength="100" showValue="0" gradient="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>